<commit_message>
change name aand add external formula
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/03_Inst_Analysis_Unit.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/03_Inst_Analysis_Unit.xlsx
@@ -44,32 +44,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>CREATE, MODIFY, CREATE/MODIFY, DELETE</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Analysis_Unit</t>
   </si>
@@ -137,9 +113,6 @@
     <t>AnalyticalTable</t>
   </si>
   <si>
-    <t>TargetVariable</t>
-  </si>
-  <si>
     <t>SNDG</t>
   </si>
   <si>
@@ -191,9 +164,6 @@
     <t>CUSTOMER</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>CUSTOMER_SNDG</t>
   </si>
   <si>
@@ -258,6 +228,15 @@
   </si>
   <si>
     <t>BACK_TESTING_V</t>
+  </si>
+  <si>
+    <t>Counterparty</t>
+  </si>
+  <si>
+    <t>OUTPUT_IRIS_WEB</t>
+  </si>
+  <si>
+    <t>LIB_EWS_IT.ExternalInfo();</t>
   </si>
 </sst>
 </file>
@@ -360,8 +339,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -386,150 +365,6 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
@@ -994,24 +829,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1023,9 +861,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1042,49 +879,48 @@
         <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>62</v>
       </c>
-      <c r="G3" t="s">
-        <v>24</v>
+      <c r="I3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1139,16 +975,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1156,16 +992,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1173,16 +1009,16 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1190,16 +1026,16 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1207,16 +1043,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1224,16 +1060,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1241,16 +1077,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1258,16 +1094,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1275,16 +1111,16 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1292,16 +1128,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1309,16 +1145,16 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1326,16 +1162,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1343,16 +1179,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1360,16 +1196,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1377,16 +1213,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
@@ -1394,16 +1230,16 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Store Intermediate Results = TRUE
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/03_Inst_Analysis_Unit.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/03_Inst_Analysis_Unit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16635" yWindow="0" windowWidth="18315" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="16635" yWindow="0" windowWidth="18315" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis_Unit" sheetId="1" r:id="rId1"/>
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,6 +1551,9 @@
       <c r="G3" t="s">
         <v>62</v>
       </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
       <c r="I3" t="s">
         <v>68</v>
       </c>
@@ -1569,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A154" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>

</xml_diff>